<commit_message>
Adicionando cenários para as histórias 8 - 13 - 7
</commit_message>
<xml_diff>
--- a/docs/testes-integracao.xlsx
+++ b/docs/testes-integracao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibrasilcombr-my.sharepoint.com/personal/2019102845_unibrasil_com_br/Documents/Facul/PP-Dev-Qualidade/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Caca-Curso_Back-end\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D802F92-7D95-4192-A980-C4A705CA0DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A077C2CD-245F-4AE6-8212-F4DA6699B16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BD6947E-446F-41CB-AC53-A68FE1B4C46F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>História</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t>Pendente</t>
+  </si>
+  <si>
+    <t>7 - Permitir o usuário avaliar com gostei/não gostei</t>
+  </si>
+  <si>
+    <t>13 - Permitir o usuário favoritar cursos</t>
+  </si>
+  <si>
+    <t>8 - Permitir o usuário avaliar um curso com comentário</t>
+  </si>
+  <si>
+    <t>Clicando no curso após a pesquisa, foi mostrado a tela de detalhes do curso, na caixa de texto disponível, foi digitado o comentário e ao postar, a tela foi atualizada mostrando o comentário e todos os outros que o curso possuia</t>
+  </si>
+  <si>
+    <t>Ao clicar em um curso, depois da pesquisa ser efetuada, o usuário é redirecionado para a página dos detalhes do curso, onde estará disponível para ele uma caixa de texto e um botão para submeter o comentário, após a realização do mesmo, a tela é atualizada com o comentário recém postado e os demais</t>
+  </si>
+  <si>
+    <t>Ao clicar em um curso, depois da pesquisa ser efetuada, o usuário é redirecionado para a página dos detalhes do curso, tela esta que deve disponibilizar o botão para o usuário favoritar o curso que está na tela</t>
+  </si>
+  <si>
+    <t>Clicando no curso após a pesquisa, foi mostrado a tela de detalhes do curso, e também o botão para favoritar o curso</t>
+  </si>
+  <si>
+    <t>Ao clicar na aba de cursos favoritados o aplicativo deve listar todos os cursos que o usuário logado favoritou e se não tiver usuário logado, sugerir para que faça o login</t>
+  </si>
+  <si>
+    <t>Indo na aba de cursos favoritados, foi listado todos que o usuário logado favoritou e sem login foi sugerido para que o usuário o faça</t>
   </si>
 </sst>
 </file>
@@ -489,15 +516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E945CD8-3F0F-4490-AB5B-0B175001DCE7}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="75.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="73.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="3" customWidth="1"/>
@@ -574,6 +601,72 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>